<commit_message>
minor changes so scripts work after Sam's updates
</commit_message>
<xml_diff>
--- a/9_parent_weight/doc/summary_table.xlsx
+++ b/9_parent_weight/doc/summary_table.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akbaldwi\Documents\GLRI\PAHs\pah\pah_glri\9_parent_weight\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E67DE913-238A-4B1C-B968-FB3D2113E45D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BFEAA77-C2DD-4DC6-A658-066A2ACB7134}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18540" windowHeight="2830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23750" windowHeight="10220"/>
   </bookViews>
   <sheets>
     <sheet name="summary_table" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>unique_id</t>
   </si>
@@ -260,37 +260,12 @@
   </si>
   <si>
     <t>WI-WMC</t>
-  </si>
-  <si>
-    <t>min</t>
-  </si>
-  <si>
-    <t xml:space="preserve">median </t>
-  </si>
-  <si>
-    <t>mean</t>
-  </si>
-  <si>
-    <t>sd</t>
-  </si>
-  <si>
-    <t>max</t>
-  </si>
-  <si>
-    <t>pct &gt; 1</t>
-  </si>
-  <si>
-    <t>pct &lt; 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -768,10 +743,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1126,14 +1099,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H84"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1160" topLeftCell="A10" activePane="bottomLeft"/>
-      <selection activeCell="D1" sqref="D1:E1048576"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1183,10 +1152,10 @@
         <v>1.2</v>
       </c>
       <c r="G2">
-        <v>3.9</v>
+        <v>2.1</v>
       </c>
       <c r="H2">
-        <v>3.3</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1209,10 +1178,10 @@
         <v>0.8</v>
       </c>
       <c r="G3">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1235,10 +1204,10 @@
         <v>6.8</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="H4">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1261,10 +1230,10 @@
         <v>0.5</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="H5">
-        <v>4.9000000000000004</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1287,10 +1256,10 @@
         <v>0.5</v>
       </c>
       <c r="G6">
-        <v>4.2</v>
+        <v>2</v>
       </c>
       <c r="H6">
-        <v>5.6</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1313,10 +1282,10 @@
         <v>0.1</v>
       </c>
       <c r="G7">
-        <v>8.1</v>
+        <v>4.8</v>
       </c>
       <c r="H7">
-        <v>6</v>
+        <v>7.1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1339,10 +1308,10 @@
         <v>0.1</v>
       </c>
       <c r="G8">
-        <v>5.0999999999999996</v>
+        <v>3</v>
       </c>
       <c r="H8">
-        <v>6.2</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1365,10 +1334,10 @@
         <v>1.4</v>
       </c>
       <c r="G9">
-        <v>6.8</v>
+        <v>3.6</v>
       </c>
       <c r="H9">
-        <v>7.8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1391,10 +1360,10 @@
         <v>17</v>
       </c>
       <c r="G10">
-        <v>3.3</v>
+        <v>1.7</v>
       </c>
       <c r="H10">
-        <v>6</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1417,10 +1386,10 @@
         <v>0.2</v>
       </c>
       <c r="G11">
-        <v>5.5</v>
+        <v>3.1</v>
       </c>
       <c r="H11">
-        <v>8.5</v>
+        <v>10.1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1443,10 +1412,10 @@
         <v>0.2</v>
       </c>
       <c r="G12">
-        <v>4</v>
+        <v>1.8</v>
       </c>
       <c r="H12">
-        <v>5.7</v>
+        <v>6.9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1469,10 +1438,10 @@
         <v>1.4</v>
       </c>
       <c r="G13">
-        <v>3.7</v>
+        <v>2</v>
       </c>
       <c r="H13">
-        <v>4.8</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1495,7 +1464,7 @@
         <v>0.6</v>
       </c>
       <c r="G14">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H14">
         <v>0.5</v>
@@ -1521,10 +1490,10 @@
         <v>0.9</v>
       </c>
       <c r="G15">
-        <v>7.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H15">
-        <v>4.0999999999999996</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1547,10 +1516,10 @@
         <v>0.3</v>
       </c>
       <c r="G16">
+        <v>0.4</v>
+      </c>
+      <c r="H16">
         <v>1.4</v>
-      </c>
-      <c r="H16">
-        <v>1.3</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1573,10 +1542,10 @@
         <v>1.6</v>
       </c>
       <c r="G17">
+        <v>2.5</v>
+      </c>
+      <c r="H17">
         <v>5.3</v>
-      </c>
-      <c r="H17">
-        <v>4.5</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1599,10 +1568,10 @@
         <v>0.1</v>
       </c>
       <c r="G18">
-        <v>7</v>
+        <v>4.2</v>
       </c>
       <c r="H18">
-        <v>4.8</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1625,10 +1594,10 @@
         <v>1.2</v>
       </c>
       <c r="G19">
-        <v>3.8</v>
+        <v>2.1</v>
       </c>
       <c r="H19">
-        <v>4.0999999999999996</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1651,10 +1620,10 @@
         <v>0.7</v>
       </c>
       <c r="G20">
-        <v>6.9</v>
+        <v>3.8</v>
       </c>
       <c r="H20">
-        <v>4.5999999999999996</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1677,10 +1646,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G21">
-        <v>8.1999999999999993</v>
+        <v>3.8</v>
       </c>
       <c r="H21">
-        <v>11</v>
+        <v>12.1</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1703,10 +1672,10 @@
         <v>0.4</v>
       </c>
       <c r="G22">
-        <v>6.8</v>
+        <v>3.7</v>
       </c>
       <c r="H22">
-        <v>5.4</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1729,10 +1698,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="G23">
-        <v>4.0999999999999996</v>
+        <v>1.8</v>
       </c>
       <c r="H23">
-        <v>5.2</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1755,10 +1724,10 @@
         <v>0.8</v>
       </c>
       <c r="G24">
-        <v>4.0999999999999996</v>
+        <v>2.1</v>
       </c>
       <c r="H24">
-        <v>5.3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1781,10 +1750,10 @@
         <v>0.4</v>
       </c>
       <c r="G25">
-        <v>8.4</v>
+        <v>4.7</v>
       </c>
       <c r="H25">
-        <v>3.9</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1807,10 +1776,10 @@
         <v>1.4</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H26">
-        <v>1.3</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1833,10 +1802,10 @@
         <v>0.4</v>
       </c>
       <c r="G27">
-        <v>5.9</v>
+        <v>3.4</v>
       </c>
       <c r="H27">
-        <v>4.0999999999999996</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1859,10 +1828,10 @@
         <v>1.4</v>
       </c>
       <c r="G28">
-        <v>2.1</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1885,10 +1854,10 @@
         <v>2.8</v>
       </c>
       <c r="G29">
-        <v>6.7</v>
+        <v>3.8</v>
       </c>
       <c r="H29">
-        <v>3.9</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1911,10 +1880,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G30">
-        <v>2.5</v>
+        <v>0.7</v>
       </c>
       <c r="H30">
-        <v>3.6</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1937,10 +1906,10 @@
         <v>3.9</v>
       </c>
       <c r="G31">
-        <v>5</v>
+        <v>2.6</v>
       </c>
       <c r="H31">
-        <v>4.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1963,10 +1932,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="G32">
-        <v>6.9</v>
+        <v>3.8</v>
       </c>
       <c r="H32">
-        <v>4.7</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1989,10 +1958,10 @@
         <v>0.3</v>
       </c>
       <c r="G33">
-        <v>2.2000000000000002</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H33">
-        <v>3.6</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2015,10 +1984,10 @@
         <v>5</v>
       </c>
       <c r="G34">
-        <v>4.5999999999999996</v>
+        <v>2.4</v>
       </c>
       <c r="H34">
-        <v>4.9000000000000004</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2041,10 +2010,10 @@
         <v>0.7</v>
       </c>
       <c r="G35">
-        <v>5.0999999999999996</v>
+        <v>2.5</v>
       </c>
       <c r="H35">
-        <v>8.6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2067,10 +2036,10 @@
         <v>2</v>
       </c>
       <c r="G36">
-        <v>7.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H36">
-        <v>7.2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2093,10 +2062,10 @@
         <v>0.3</v>
       </c>
       <c r="G37">
-        <v>4.5999999999999996</v>
+        <v>2.4</v>
       </c>
       <c r="H37">
-        <v>5.2</v>
+        <v>5.7</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2119,10 +2088,10 @@
         <v>0.6</v>
       </c>
       <c r="G38">
-        <v>4.3</v>
+        <v>3.5</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2145,10 +2114,10 @@
         <v>0.4</v>
       </c>
       <c r="G39">
-        <v>4.8</v>
+        <v>2.4</v>
       </c>
       <c r="H39">
-        <v>6.6</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -2171,10 +2140,10 @@
         <v>0.1</v>
       </c>
       <c r="G40">
-        <v>5.4</v>
+        <v>2.9</v>
       </c>
       <c r="H40">
-        <v>3.5</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2197,7 +2166,7 @@
         <v>0.7</v>
       </c>
       <c r="G41">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H41">
         <v>0.3</v>
@@ -2223,10 +2192,10 @@
         <v>0.4</v>
       </c>
       <c r="G42">
-        <v>2.2000000000000002</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H42">
-        <v>3.7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2275,10 +2244,10 @@
         <v>1.4</v>
       </c>
       <c r="G44">
+        <v>0.6</v>
+      </c>
+      <c r="H44">
         <v>0.9</v>
-      </c>
-      <c r="H44">
-        <v>0.8</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -2301,10 +2270,10 @@
         <v>1</v>
       </c>
       <c r="G45">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H45">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -2327,10 +2296,10 @@
         <v>0.5</v>
       </c>
       <c r="G46">
-        <v>1.6</v>
+        <v>0.4</v>
       </c>
       <c r="H46">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -2353,10 +2322,10 @@
         <v>1.4</v>
       </c>
       <c r="G47">
-        <v>3.9</v>
+        <v>2.1</v>
       </c>
       <c r="H47">
-        <v>3.8</v>
+        <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -2379,10 +2348,10 @@
         <v>0.6</v>
       </c>
       <c r="G48">
+        <v>0.3</v>
+      </c>
+      <c r="H48">
         <v>0.5</v>
-      </c>
-      <c r="H48">
-        <v>0.4</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -2405,7 +2374,7 @@
         <v>0.5</v>
       </c>
       <c r="G49">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="H49">
         <v>0.3</v>
@@ -2431,10 +2400,10 @@
         <v>1.9</v>
       </c>
       <c r="G50">
-        <v>1.4</v>
+        <v>0.9</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -2457,10 +2426,10 @@
         <v>1.8</v>
       </c>
       <c r="G51">
-        <v>6.1</v>
+        <v>2.9</v>
       </c>
       <c r="H51">
-        <v>11.8</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -2468,7 +2437,7 @@
         <v>59</v>
       </c>
       <c r="B52">
-        <v>7.42</v>
+        <v>7</v>
       </c>
       <c r="C52">
         <v>0</v>
@@ -2483,10 +2452,10 @@
         <v>0.3</v>
       </c>
       <c r="G52">
-        <v>11</v>
+        <v>2.4</v>
       </c>
       <c r="H52">
-        <v>11.4</v>
+        <v>13.9</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -2509,10 +2478,10 @@
         <v>2.5</v>
       </c>
       <c r="G53">
-        <v>4.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H53">
-        <v>6.9</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -2535,10 +2504,10 @@
         <v>0.3</v>
       </c>
       <c r="G54">
-        <v>5.0999999999999996</v>
+        <v>2.6</v>
       </c>
       <c r="H54">
-        <v>9.1999999999999993</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -2561,10 +2530,10 @@
         <v>2.4</v>
       </c>
       <c r="G55">
-        <v>6.2</v>
+        <v>3.5</v>
       </c>
       <c r="H55">
-        <v>4.5</v>
+        <v>5.0999999999999996</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
@@ -2587,10 +2556,10 @@
         <v>3.8</v>
       </c>
       <c r="G56">
-        <v>3.3</v>
+        <v>1.8</v>
       </c>
       <c r="H56">
-        <v>4.2</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
@@ -2613,10 +2582,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G57">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="H57">
-        <v>1.2</v>
+        <v>1.4</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -2639,10 +2608,10 @@
         <v>2.8</v>
       </c>
       <c r="G58">
-        <v>5.5</v>
+        <v>2.9</v>
       </c>
       <c r="H58">
-        <v>5.3</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
@@ -2665,10 +2634,10 @@
         <v>2</v>
       </c>
       <c r="G59">
-        <v>6.6</v>
+        <v>3.5</v>
       </c>
       <c r="H59">
-        <v>5.4</v>
+        <v>5.9</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
@@ -2691,10 +2660,10 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="G60">
-        <v>2.6</v>
+        <v>1.2</v>
       </c>
       <c r="H60">
-        <v>3.5</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
@@ -2717,10 +2686,10 @@
         <v>2.1</v>
       </c>
       <c r="G61">
-        <v>6.6</v>
+        <v>3.4</v>
       </c>
       <c r="H61">
-        <v>5.7</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -2743,10 +2712,10 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="G62">
-        <v>6.6</v>
+        <v>3.4</v>
       </c>
       <c r="H62">
-        <v>4.9000000000000004</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -2769,10 +2738,10 @@
         <v>2.1</v>
       </c>
       <c r="G63">
-        <v>3.7</v>
+        <v>2</v>
       </c>
       <c r="H63">
-        <v>4.2</v>
+        <v>4.5999999999999996</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
@@ -2795,10 +2764,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="G64">
-        <v>4.5</v>
+        <v>2.4</v>
       </c>
       <c r="H64">
-        <v>5</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
@@ -2821,10 +2790,10 @@
         <v>7</v>
       </c>
       <c r="G65">
-        <v>5.4</v>
+        <v>2.7</v>
       </c>
       <c r="H65">
-        <v>7.3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
@@ -2847,10 +2816,10 @@
         <v>0.7</v>
       </c>
       <c r="G66">
-        <v>7.1</v>
+        <v>3.6</v>
       </c>
       <c r="H66">
-        <v>11</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
@@ -2873,10 +2842,10 @@
         <v>1.6</v>
       </c>
       <c r="G67">
-        <v>5.0999999999999996</v>
+        <v>2.8</v>
       </c>
       <c r="H67">
-        <v>4.4000000000000004</v>
+        <v>4.9000000000000004</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -2899,10 +2868,10 @@
         <v>4.2</v>
       </c>
       <c r="G68">
-        <v>4.9000000000000004</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H68">
-        <v>6.4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
@@ -2925,10 +2894,10 @@
         <v>0.7</v>
       </c>
       <c r="G69">
-        <v>5.4</v>
+        <v>2.9</v>
       </c>
       <c r="H69">
-        <v>6.6</v>
+        <v>7.3</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
@@ -2951,10 +2920,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G70">
-        <v>4</v>
+        <v>1.9</v>
       </c>
       <c r="H70">
-        <v>6.9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
@@ -2977,10 +2946,10 @@
         <v>2.1</v>
       </c>
       <c r="G71">
-        <v>7.6</v>
+        <v>4</v>
       </c>
       <c r="H71">
-        <v>5.0999999999999996</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
@@ -3003,245 +2972,10 @@
         <v>2</v>
       </c>
       <c r="G72">
-        <v>4.0999999999999996</v>
+        <v>2</v>
       </c>
       <c r="H72">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74" s="2">
-        <f>MIN(B2:B72)</f>
-        <v>7.42</v>
-      </c>
-      <c r="C74">
-        <f t="shared" ref="C74:H74" si="0">MIN(C2:C72)</f>
-        <v>0</v>
-      </c>
-      <c r="D74">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E74">
-        <f t="shared" si="0"/>
-        <v>0.01</v>
-      </c>
-      <c r="F74">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="G74">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="H74">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>81</v>
-      </c>
-      <c r="B75">
-        <f>MEDIAN(B2:B72)</f>
-        <v>2603</v>
-      </c>
-      <c r="C75">
-        <f t="shared" ref="C75:H75" si="1">MEDIAN(C2:C72)</f>
-        <v>1.62</v>
-      </c>
-      <c r="D75">
-        <f t="shared" si="1"/>
-        <v>0.11</v>
-      </c>
-      <c r="E75">
-        <f t="shared" si="1"/>
-        <v>0.44</v>
-      </c>
-      <c r="F75">
-        <f t="shared" si="1"/>
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="G75">
-        <f t="shared" si="1"/>
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="H75">
-        <f t="shared" si="1"/>
-        <v>4.7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>82</v>
-      </c>
-      <c r="B76">
-        <f>AVERAGE(B2:B72)</f>
-        <v>13328.653802816902</v>
-      </c>
-      <c r="C76">
-        <f t="shared" ref="C76:H76" si="2">AVERAGE(C2:C72)</f>
-        <v>8.2787323943661946</v>
-      </c>
-      <c r="D76">
-        <f t="shared" si="2"/>
-        <v>0.58408450704225345</v>
-      </c>
-      <c r="E76">
-        <f t="shared" si="2"/>
-        <v>1.2590000000000001</v>
-      </c>
-      <c r="F76">
-        <f t="shared" si="2"/>
-        <v>1.675714285714285</v>
-      </c>
-      <c r="G76">
-        <f t="shared" si="2"/>
-        <v>4.3746478873239436</v>
-      </c>
-      <c r="H76">
-        <f t="shared" si="2"/>
-        <v>4.6535211267605616</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>83</v>
-      </c>
-      <c r="B77">
-        <f>STDEV(B2:B72)</f>
-        <v>29803.88358303731</v>
-      </c>
-      <c r="C77">
-        <f t="shared" ref="C77:H77" si="3">STDEV(C2:C72)</f>
-        <v>18.511859899579239</v>
-      </c>
-      <c r="D77">
-        <f t="shared" si="3"/>
-        <v>1.3079881797901787</v>
-      </c>
-      <c r="E77">
-        <f t="shared" si="3"/>
-        <v>1.7965806088394618</v>
-      </c>
-      <c r="F77">
-        <f t="shared" si="3"/>
-        <v>1.7512261306474757</v>
-      </c>
-      <c r="G77">
-        <f t="shared" si="3"/>
-        <v>2.4116809970201945</v>
-      </c>
-      <c r="H77">
-        <f t="shared" si="3"/>
-        <v>2.721282837503328</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>84</v>
-      </c>
-      <c r="B78">
-        <f>MAX(B2:B72)</f>
-        <v>195788</v>
-      </c>
-      <c r="C78">
-        <f t="shared" ref="C78:H78" si="4">MAX(C2:C72)</f>
-        <v>121.61</v>
-      </c>
-      <c r="D78">
-        <f t="shared" si="4"/>
-        <v>8.59</v>
-      </c>
-      <c r="E78">
-        <f t="shared" si="4"/>
-        <v>10.47</v>
-      </c>
-      <c r="F78">
-        <f t="shared" si="4"/>
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="G78">
-        <f t="shared" si="4"/>
-        <v>11</v>
-      </c>
-      <c r="H78">
-        <f t="shared" si="4"/>
-        <v>11.8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>85</v>
-      </c>
-      <c r="C80" s="1">
-        <f t="shared" ref="C80:H80" si="5">(COUNTIF(C2:C72,"&gt;1")/71)*100</f>
-        <v>61.971830985915489</v>
-      </c>
-      <c r="D80" s="1">
-        <f t="shared" si="5"/>
-        <v>18.30985915492958</v>
-      </c>
-      <c r="E80" s="1">
-        <f t="shared" si="5"/>
-        <v>38.028169014084504</v>
-      </c>
-      <c r="F80" s="1">
-        <f t="shared" si="5"/>
-        <v>53.521126760563376</v>
-      </c>
-      <c r="G80" s="1">
-        <f t="shared" si="5"/>
-        <v>84.507042253521121</v>
-      </c>
-      <c r="H80" s="1">
-        <f t="shared" si="5"/>
-        <v>85.91549295774648</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
-        <v>86</v>
-      </c>
-      <c r="C81" s="1">
-        <f>(COUNTIF(C2:C72,"&lt;1")/71)*100</f>
-        <v>38.028169014084504</v>
-      </c>
-      <c r="D81" s="1">
-        <f t="shared" ref="D81:H81" si="6">(COUNTIF(D2:D72,"&lt;1")/71)*100</f>
-        <v>81.690140845070431</v>
-      </c>
-      <c r="E81" s="1">
-        <f t="shared" si="6"/>
-        <v>60.563380281690137</v>
-      </c>
-      <c r="F81" s="1">
-        <f t="shared" si="6"/>
-        <v>43.661971830985912</v>
-      </c>
-      <c r="G81" s="1">
-        <f t="shared" si="6"/>
-        <v>12.676056338028168</v>
-      </c>
-      <c r="H81" s="1">
-        <f t="shared" si="6"/>
-        <v>9.8591549295774641</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E83">
-        <f>29/71</f>
-        <v>0.40845070422535212</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="E84">
-        <f>27/71</f>
-        <v>0.38028169014084506</v>
+        <v>5.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>